<commit_message>
golden zone kpi done
</commit_message>
<xml_diff>
--- a/Projects/PNGJP_SAND2/Data/TemplateBlockAndGoldenZoneKPI.xlsx
+++ b/Projects/PNGJP_SAND2/Data/TemplateBlockAndGoldenZoneKPI.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Block" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="147">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -1177,10 +1177,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:AMJ5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1379,6 +1379,46 @@
       </c>
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>4902135142500</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="P5" s="7" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="AMG5" s="0"/>
+      <c r="AMH5" s="0"/>
+      <c r="AMI5" s="0"/>
+      <c r="AMJ5" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3460,8 +3500,8 @@
   </sheetPr>
   <dimension ref="A1:W6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3763,6 +3803,9 @@
       </c>
       <c r="F6" s="1" t="s">
         <v>127</v>
+      </c>
+      <c r="O6" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="P6" s="54" t="n">
         <v>0.8</v>

</xml_diff>